<commit_message>
implementar seleção e renomeio de pasta na  arvore
</commit_message>
<xml_diff>
--- a/BdaC_ProAtiv.xlsx
+++ b/BdaC_ProAtiv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Projetos4\Desktop\ALESSANDRO\MACRO\Criando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F62D5EE-57E1-4506-B9EB-D78455C32FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE9681E-14A9-435E-A145-1E97F12D0E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,13 +560,13 @@
     <t>CONJ. SOLDADO</t>
   </si>
   <si>
-    <t>CASO</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>thread</t>
+  </si>
+  <si>
+    <t>CLASSE</t>
   </si>
 </sst>
 </file>
@@ -831,11 +831,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:Y111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1157,51 +1157,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="X2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Iniciando a conexão com o BDA e criando propriedades de acordo com o banco
</commit_message>
<xml_diff>
--- a/BdaC_ProAtiv.xlsx
+++ b/BdaC_ProAtiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Projetos4\Desktop\ALESSANDRO\MACRO\Criando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE9681E-14A9-435E-A145-1E97F12D0E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB3854A-43D5-40E2-87BB-B1142A7615D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="181">
   <si>
     <t>DESCRIÇÃO DECISAO</t>
   </si>
@@ -567,6 +567,12 @@
   </si>
   <si>
     <t>CLASSE</t>
+  </si>
+  <si>
+    <t>FIM FUNDIDOS</t>
+  </si>
+  <si>
+    <t>FIM SOLDADOS</t>
   </si>
 </sst>
 </file>
@@ -685,7 +691,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -743,6 +749,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,7 +835,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -836,6 +848,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1138,7 +1152,7 @@
   <dimension ref="A1:Y111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1380,6 +1394,13 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:25" s="8" customFormat="1">
+      <c r="A11" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+    </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>152</v>
@@ -1413,6 +1434,9 @@
       <c r="D13" t="s">
         <v>174</v>
       </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
       <c r="J13">
         <v>2</v>
       </c>
@@ -1430,6 +1454,9 @@
       <c r="D14" t="s">
         <v>174</v>
       </c>
+      <c r="E14" t="s">
+        <v>175</v>
+      </c>
       <c r="J14">
         <v>2</v>
       </c>
@@ -1447,6 +1474,9 @@
       <c r="D15" t="s">
         <v>174</v>
       </c>
+      <c r="E15" t="s">
+        <v>175</v>
+      </c>
       <c r="J15">
         <v>2</v>
       </c>
@@ -1464,6 +1494,9 @@
       <c r="D16" t="s">
         <v>174</v>
       </c>
+      <c r="E16" t="s">
+        <v>175</v>
+      </c>
       <c r="J16">
         <v>2</v>
       </c>
@@ -1481,6 +1514,16 @@
       <c r="D17" t="s">
         <v>174</v>
       </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" s="8" customFormat="1">
+      <c r="A18" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">

</xml_diff>

<commit_message>
Inicio de projeto para classe peça
</commit_message>
<xml_diff>
--- a/BdaC_ProAtiv.xlsx
+++ b/BdaC_ProAtiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Projetos4\Desktop\ALESSANDRO\MACRO\Criando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB3854A-43D5-40E2-87BB-B1142A7615D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A9C4F0-95C9-45C5-95F4-538748367EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="181">
-  <si>
-    <t>DESCRIÇÃO DECISAO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="188">
   <si>
     <t>MATERIAL</t>
   </si>
@@ -557,15 +554,9 @@
     <t>CALCULADO</t>
   </si>
   <si>
-    <t>CONJ. SOLDADO</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>thread</t>
-  </si>
-  <si>
     <t>CLASSE</t>
   </si>
   <si>
@@ -573,6 +564,36 @@
   </si>
   <si>
     <t>FIM SOLDADOS</t>
+  </si>
+  <si>
+    <t>SOLD_COMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LACHA;CALÇO;MUNHÃO </t>
+  </si>
+  <si>
+    <t>CFME_ESP</t>
+  </si>
+  <si>
+    <t>BASE FIXAÇÃO;CALÇO</t>
+  </si>
+  <si>
+    <t>ENTRADA TIRA SOLD.</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>MESA ENTRADA TIRA;FIXAÇÃO TIRA; REFORÇO</t>
+  </si>
+  <si>
+    <t>BASE SENSOR;SUPORTE</t>
+  </si>
+  <si>
+    <t>PINO ENCOSTO;BASE FIXAÇÃO</t>
+  </si>
+  <si>
+    <t>DENOMINAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -759,7 +780,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -812,6 +833,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -835,7 +867,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -845,11 +877,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1149,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y111"/>
+  <dimension ref="A1:Y112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1166,76 +1199,78 @@
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="41.5703125" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="18" max="18" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>3</v>
-      </c>
       <c r="H2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>177</v>
-      </c>
+      <c r="L2" s="5"/>
       <c r="X2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3">
@@ -1245,24 +1280,24 @@
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Y3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1271,24 +1306,24 @@
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1296,19 +1331,19 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1316,19 +1351,19 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1336,19 +1371,19 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1356,19 +1391,19 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1376,129 +1411,159 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="8" customFormat="1">
-      <c r="A11" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+    <row r="11" spans="1:25" s="7" customFormat="1">
+      <c r="A11" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E12" t="s">
-        <v>175</v>
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
       </c>
       <c r="J12">
         <v>2</v>
       </c>
+      <c r="K12" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>175</v>
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
       </c>
       <c r="J13">
         <v>2</v>
       </c>
+      <c r="K13" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E14" t="s">
-        <v>175</v>
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
+      <c r="K14" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
       </c>
       <c r="J15">
         <v>2</v>
       </c>
+      <c r="K15" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>175</v>
+        <v>180</v>
+      </c>
+      <c r="F16" t="s">
+        <v>180</v>
       </c>
       <c r="J16">
         <v>2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -1506,364 +1571,381 @@
         <v>156</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
         <v>173</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
-        <v>174</v>
-      </c>
       <c r="E17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" s="8" customFormat="1">
-      <c r="A18" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:25">
-      <c r="A19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="J19">
+      <c r="F17" t="s">
+        <v>180</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" t="s">
+        <v>180</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" s="7" customFormat="1">
+      <c r="A19" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
-      <c r="R20" t="s">
+    <row r="21" spans="1:25">
+      <c r="R21" t="s">
+        <v>8</v>
+      </c>
+      <c r="S21" t="s">
         <v>9</v>
       </c>
-      <c r="S20" t="s">
-        <v>10</v>
-      </c>
-      <c r="T20" t="s">
-        <v>8</v>
-      </c>
-      <c r="U20" t="s">
-        <v>133</v>
-      </c>
-      <c r="X20" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y20" t="s">
+      <c r="T21" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" t="s">
+        <v>132</v>
+      </c>
+      <c r="X21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="R29" t="s">
+        <v>48</v>
+      </c>
+      <c r="S29" t="s">
+        <v>3</v>
+      </c>
+      <c r="T29" t="s">
+        <v>17</v>
+      </c>
+      <c r="U29" t="s">
+        <v>49</v>
+      </c>
+      <c r="X29" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y29" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
-      <c r="R28" t="s">
-        <v>49</v>
-      </c>
-      <c r="S28" t="s">
-        <v>4</v>
-      </c>
-      <c r="T28" t="s">
-        <v>18</v>
-      </c>
-      <c r="U28" t="s">
-        <v>50</v>
-      </c>
-      <c r="X28" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="R29" t="s">
-        <v>51</v>
-      </c>
-      <c r="S29" t="s">
-        <v>7</v>
-      </c>
-      <c r="T29" t="s">
-        <v>18</v>
-      </c>
-      <c r="U29" t="s">
-        <v>50</v>
-      </c>
-      <c r="X29" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="R30" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="S30" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="T30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X30" t="s">
-        <v>88</v>
+        <v>25</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:25">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>51</v>
       </c>
       <c r="R31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="S31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T31" t="s">
-        <v>22</v>
-      </c>
-      <c r="V31" t="str">
+        <v>17</v>
+      </c>
+      <c r="U31" t="s">
+        <v>49</v>
+      </c>
+      <c r="X31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="R32" t="s">
+        <v>72</v>
+      </c>
+      <c r="S32" t="s">
+        <v>70</v>
+      </c>
+      <c r="T32" t="s">
+        <v>21</v>
+      </c>
+      <c r="V32" t="str">
         <f>$Y$3</f>
         <v>T.R 54-56 Hrc</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
-      <c r="A32" t="s">
-        <v>145</v>
-      </c>
-      <c r="R32" t="s">
-        <v>72</v>
-      </c>
-      <c r="S32" t="s">
-        <v>72</v>
-      </c>
-      <c r="T32" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="33" spans="1:24">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="S33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="T33" t="s">
-        <v>22</v>
-      </c>
-      <c r="V33" t="str">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="R34" t="s">
+        <v>73</v>
+      </c>
+      <c r="S34" t="s">
+        <v>71</v>
+      </c>
+      <c r="T34" t="s">
+        <v>21</v>
+      </c>
+      <c r="V34" t="str">
         <f>$Y$3</f>
         <v>T.R 54-56 Hrc</v>
       </c>
-      <c r="X33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24">
-      <c r="A34" t="s">
-        <v>147</v>
-      </c>
-      <c r="R34" t="s">
-        <v>53</v>
-      </c>
-      <c r="S34" t="s">
-        <v>52</v>
-      </c>
-      <c r="T34" t="s">
-        <v>18</v>
-      </c>
-      <c r="U34" t="s">
-        <v>50</v>
-      </c>
       <c r="X34" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:24">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="R35" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="S35" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="T35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X35" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:24">
       <c r="A36" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="R36" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="S36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U36" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="X36" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:24">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="R37" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="T37" t="s">
+        <v>17</v>
+      </c>
+      <c r="U37" t="s">
         <v>18</v>
       </c>
-      <c r="U37" t="s">
-        <v>19</v>
-      </c>
       <c r="X37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:24">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="R38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="S38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="T38" t="s">
+        <v>17</v>
+      </c>
+      <c r="U38" t="s">
         <v>18</v>
       </c>
-      <c r="U38" t="s">
-        <v>19</v>
-      </c>
       <c r="X38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="A39" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="R39" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="S39" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="T39" t="s">
+        <v>17</v>
+      </c>
+      <c r="U39" t="s">
         <v>18</v>
       </c>
       <c r="X39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R40" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="S40" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="T40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X40" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:24">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
       <c r="R41" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="S41" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="T41" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="X41" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:24">
       <c r="R42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="S42" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T42" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="X42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:24">
       <c r="R43" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="S43" t="s">
+        <v>85</v>
       </c>
       <c r="T43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:24">
       <c r="R44" t="s">
-        <v>77</v>
-      </c>
-      <c r="S44" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="T44" t="s">
-        <v>25</v>
-      </c>
-      <c r="V44" t="str">
-        <f>$Y$28</f>
-        <v>C.T.R 60-62 Hrc</v>
+        <v>17</v>
       </c>
       <c r="X44" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:24">
@@ -1871,221 +1953,231 @@
         <v>76</v>
       </c>
       <c r="S45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="T45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="V45" t="str">
-        <f>$Y$28</f>
+        <f>$Y$29</f>
         <v>C.T.R 60-62 Hrc</v>
       </c>
       <c r="X45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:24">
       <c r="R46" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S46" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="T46" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="V46" t="str">
+        <f>$Y$29</f>
+        <v>C.T.R 60-62 Hrc</v>
       </c>
       <c r="X46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:24">
       <c r="R47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="S47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="T47" t="s">
-        <v>23</v>
-      </c>
-      <c r="V47" t="str">
-        <f>$Y$20</f>
-        <v>T.R 60-62 Hrc</v>
+        <v>28</v>
       </c>
       <c r="X47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:24">
       <c r="R48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="T48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V48" t="str">
-        <f>$Y$20</f>
+        <f>$Y$21</f>
         <v>T.R 60-62 Hrc</v>
       </c>
       <c r="X48" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:24">
       <c r="R49" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="S49" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V49" t="str">
-        <f>$Y$20</f>
+        <f>$Y$21</f>
         <v>T.R 60-62 Hrc</v>
       </c>
       <c r="X49" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" ht="51">
-      <c r="R50" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
+      <c r="R50" t="s">
+        <v>81</v>
+      </c>
+      <c r="S50" t="s">
+        <v>81</v>
+      </c>
+      <c r="T50" t="s">
+        <v>22</v>
+      </c>
+      <c r="V50" t="str">
+        <f>$Y$21</f>
+        <v>T.R 60-62 Hrc</v>
+      </c>
+      <c r="X50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" ht="51">
+      <c r="R51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T51" t="s">
         <v>17</v>
       </c>
-      <c r="S50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T50" t="s">
+      <c r="U51" t="s">
         <v>18</v>
       </c>
-      <c r="U50" t="s">
-        <v>19</v>
-      </c>
-      <c r="X50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24">
-      <c r="X51">
+      <c r="X51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24">
+      <c r="X52">
         <v>1.2768999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24">
-      <c r="R52" t="s">
-        <v>54</v>
-      </c>
-      <c r="S52" t="s">
-        <v>55</v>
-      </c>
-      <c r="T52" t="str">
-        <f>$X$43</f>
-        <v>PRODTY</v>
       </c>
     </row>
     <row r="53" spans="1:24">
       <c r="R53" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="S53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T53" t="str">
         <f>$X$44</f>
-        <v>KALLER</v>
+        <v>PRODTY</v>
       </c>
     </row>
     <row r="54" spans="1:24">
       <c r="R54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T54" t="str">
-        <f>$X$46</f>
-        <v>AZOL GAS</v>
+        <f>$X$45</f>
+        <v>KALLER</v>
       </c>
     </row>
     <row r="55" spans="1:24">
       <c r="R55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T55" t="str">
-        <f>$X$45</f>
-        <v>DADCO</v>
+        <f>$X$47</f>
+        <v>AZOL GAS</v>
       </c>
     </row>
     <row r="56" spans="1:24">
       <c r="R56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S56" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="T56" t="str">
-        <f>$X$43</f>
-        <v>PRODTY</v>
+        <f>$X$46</f>
+        <v>DADCO</v>
       </c>
     </row>
     <row r="57" spans="1:24">
       <c r="R57" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T57" t="str">
         <f>$X$44</f>
-        <v>KALLER</v>
+        <v>PRODTY</v>
       </c>
     </row>
     <row r="58" spans="1:24">
       <c r="R58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T58" t="str">
-        <f>$X$46</f>
-        <v>AZOL GAS</v>
+        <f>$X$45</f>
+        <v>KALLER</v>
       </c>
     </row>
     <row r="59" spans="1:24">
       <c r="R59" t="s">
+        <v>60</v>
+      </c>
+      <c r="S59" t="s">
         <v>62</v>
       </c>
-      <c r="S59" t="s">
-        <v>63</v>
-      </c>
       <c r="T59" t="str">
-        <f>$X$45</f>
+        <f>$X$47</f>
+        <v>AZOL GAS</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24">
+      <c r="R60" t="s">
+        <v>61</v>
+      </c>
+      <c r="S60" t="s">
+        <v>62</v>
+      </c>
+      <c r="T60" t="str">
+        <f>$X$46</f>
         <v>DADCO</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
-      <c r="A62" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="12:13">
-      <c r="L68" s="2" t="s">
-        <v>102</v>
+    <row r="63" spans="1:24">
+      <c r="A63" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="12:13">
-      <c r="L69" t="s">
+      <c r="L69" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="M69">
-        <v>3.18</v>
       </c>
     </row>
     <row r="70" spans="12:13">
@@ -2093,7 +2185,7 @@
         <v>100</v>
       </c>
       <c r="M70">
-        <v>4.76</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="71" spans="12:13">
@@ -2101,7 +2193,7 @@
         <v>99</v>
       </c>
       <c r="M71">
-        <v>6.35</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="72" spans="12:13">
@@ -2109,7 +2201,7 @@
         <v>98</v>
       </c>
       <c r="M72">
-        <v>7.94</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="73" spans="12:13">
@@ -2117,7 +2209,7 @@
         <v>97</v>
       </c>
       <c r="M73">
-        <v>9.5299999999999994</v>
+        <v>7.94</v>
       </c>
     </row>
     <row r="74" spans="12:13">
@@ -2125,7 +2217,7 @@
         <v>96</v>
       </c>
       <c r="M74">
-        <v>12.7</v>
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="75" spans="12:13">
@@ -2133,7 +2225,7 @@
         <v>95</v>
       </c>
       <c r="M75">
-        <v>14.29</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="76" spans="12:13">
@@ -2141,7 +2233,7 @@
         <v>94</v>
       </c>
       <c r="M76">
-        <v>15.88</v>
+        <v>14.29</v>
       </c>
     </row>
     <row r="77" spans="12:13">
@@ -2149,7 +2241,7 @@
         <v>93</v>
       </c>
       <c r="M77">
-        <v>19.05</v>
+        <v>15.88</v>
       </c>
     </row>
     <row r="78" spans="12:13">
@@ -2157,7 +2249,7 @@
         <v>92</v>
       </c>
       <c r="M78">
-        <v>22.22</v>
+        <v>19.05</v>
       </c>
     </row>
     <row r="79" spans="12:13">
@@ -2165,7 +2257,7 @@
         <v>91</v>
       </c>
       <c r="M79">
-        <v>25.4</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="80" spans="12:13">
@@ -2173,7 +2265,7 @@
         <v>90</v>
       </c>
       <c r="M80">
-        <v>28.57</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="81" spans="12:13">
@@ -2181,246 +2273,254 @@
         <v>89</v>
       </c>
       <c r="M81">
-        <v>30.16</v>
+        <v>28.57</v>
       </c>
     </row>
     <row r="82" spans="12:13">
       <c r="L82" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="M82">
-        <v>31.75</v>
+        <v>30.16</v>
       </c>
     </row>
     <row r="83" spans="12:13">
       <c r="L83" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M83">
-        <v>33.340000000000003</v>
+        <v>31.75</v>
       </c>
     </row>
     <row r="84" spans="12:13">
       <c r="L84" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M84">
-        <v>34.92</v>
+        <v>33.340000000000003</v>
       </c>
     </row>
     <row r="85" spans="12:13">
       <c r="L85" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M85">
-        <v>38.1</v>
+        <v>34.92</v>
       </c>
     </row>
     <row r="86" spans="12:13">
       <c r="L86" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M86">
-        <v>39.69</v>
+        <v>38.1</v>
       </c>
     </row>
     <row r="87" spans="12:13">
       <c r="L87" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M87">
-        <v>41.27</v>
+        <v>39.69</v>
       </c>
     </row>
     <row r="88" spans="12:13">
       <c r="L88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M88">
-        <v>44.15</v>
+        <v>41.27</v>
       </c>
     </row>
     <row r="89" spans="12:13">
       <c r="L89" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M89">
-        <v>47.62</v>
+        <v>44.15</v>
       </c>
     </row>
     <row r="90" spans="12:13">
       <c r="L90" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M90">
-        <v>50.8</v>
+        <v>47.62</v>
       </c>
     </row>
     <row r="91" spans="12:13">
       <c r="L91" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M91">
-        <v>53.97</v>
+        <v>50.8</v>
       </c>
     </row>
     <row r="92" spans="12:13">
       <c r="L92" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M92">
-        <v>55.56</v>
+        <v>53.97</v>
       </c>
     </row>
     <row r="93" spans="12:13">
       <c r="L93" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M93">
-        <v>57.15</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="94" spans="12:13">
       <c r="L94" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M94">
-        <v>58.74</v>
+        <v>57.15</v>
       </c>
     </row>
     <row r="95" spans="12:13">
       <c r="L95" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M95">
-        <v>60.32</v>
+        <v>58.74</v>
       </c>
     </row>
     <row r="96" spans="12:13">
       <c r="L96" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M96">
-        <v>63.5</v>
+        <v>60.32</v>
       </c>
     </row>
     <row r="97" spans="12:13">
       <c r="L97" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M97">
-        <v>66.67</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="98" spans="12:13">
       <c r="L98" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M98">
-        <v>69.849999999999994</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="99" spans="12:13">
       <c r="L99" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M99">
-        <v>73.02</v>
+        <v>69.849999999999994</v>
       </c>
     </row>
     <row r="100" spans="12:13">
       <c r="L100" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M100">
-        <v>76.2</v>
+        <v>73.02</v>
       </c>
     </row>
     <row r="101" spans="12:13">
       <c r="L101" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M101">
-        <v>79.38</v>
+        <v>76.2</v>
       </c>
     </row>
     <row r="102" spans="12:13">
       <c r="L102" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M102">
-        <v>82.55</v>
+        <v>79.38</v>
       </c>
     </row>
     <row r="103" spans="12:13">
       <c r="L103" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M103">
-        <v>88.9</v>
+        <v>82.55</v>
       </c>
     </row>
     <row r="104" spans="12:13">
       <c r="L104" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M104">
-        <v>92.08</v>
+        <v>88.9</v>
       </c>
     </row>
     <row r="105" spans="12:13">
       <c r="L105" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M105">
-        <v>95.25</v>
+        <v>92.08</v>
       </c>
     </row>
     <row r="106" spans="12:13">
       <c r="L106" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M106">
-        <v>98.43</v>
+        <v>95.25</v>
       </c>
     </row>
     <row r="107" spans="12:13">
       <c r="L107" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M107">
-        <v>101.6</v>
+        <v>98.43</v>
       </c>
     </row>
     <row r="108" spans="12:13">
       <c r="L108" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M108">
-        <v>107.95</v>
+        <v>101.6</v>
       </c>
     </row>
     <row r="109" spans="12:13">
       <c r="L109" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M109">
-        <v>114.3</v>
+        <v>107.95</v>
       </c>
     </row>
     <row r="110" spans="12:13">
       <c r="L110" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M110">
-        <v>120.65</v>
+        <v>114.3</v>
       </c>
     </row>
     <row r="111" spans="12:13">
       <c r="L111" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M111">
+        <v>120.65</v>
+      </c>
+    </row>
+    <row r="112" spans="12:13">
+      <c r="L112" t="s">
+        <v>131</v>
+      </c>
+      <c r="M112">
         <v>127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug resolvido, Inicio de retorno valores.
</commit_message>
<xml_diff>
--- a/BdaC_ProAtiv.xlsx
+++ b/BdaC_ProAtiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Projetos4\Desktop\ALESSANDRO\MACRO\Criando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C4549-A51D-4402-845F-7AAAC319F02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119B0CC4-F498-43C5-8176-0E221D9F7434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26175" yWindow="1500" windowWidth="17100" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="245">
   <si>
     <t>MATERIAL</t>
   </si>
@@ -753,6 +753,18 @@
   </si>
   <si>
     <t>ALT +5</t>
+  </si>
+  <si>
+    <t>FIM</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>USINADO</t>
+  </si>
+  <si>
+    <t>BRUTO/USINADO</t>
   </si>
 </sst>
 </file>
@@ -883,7 +895,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -962,8 +974,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1133,6 +1151,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1156,7 +1185,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1188,6 +1217,23 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1215,9 +1261,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1227,17 +1270,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1548,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1570,21 +1602,26 @@
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" customWidth="1"/>
     <col min="17" max="17" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="5.5703125" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" customWidth="1"/>
     <col min="20" max="20" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
@@ -1630,23 +1667,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="32" customFormat="1">
+    <row r="3" spans="1:25">
       <c r="A3" s="12" t="s">
         <v>159</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="14" t="s">
@@ -1672,7 +1709,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
-      <c r="L4" s="33">
+      <c r="L4" s="19">
         <v>1</v>
       </c>
       <c r="X4" t="s">
@@ -1706,7 +1743,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="33">
+      <c r="L5" s="19">
         <v>1</v>
       </c>
       <c r="X5" t="s">
@@ -1740,7 +1777,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
-      <c r="L6" s="33">
+      <c r="L6" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1770,7 +1807,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="33">
+      <c r="L7" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1800,7 +1837,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="33">
+      <c r="L8" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1830,7 +1867,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="33">
+      <c r="L9" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1860,7 +1897,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="33">
+      <c r="L10" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1890,7 +1927,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="33">
+      <c r="L11" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1920,30 +1957,30 @@
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="33">
+      <c r="L12" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="32" customFormat="1">
+    <row r="13" spans="1:25">
       <c r="A13" s="12" t="s">
         <v>158</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="48"/>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="31" t="s">
         <v>131</v>
       </c>
       <c r="B14" s="15" t="s">
@@ -1970,7 +2007,7 @@
       <c r="K14" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="19">
         <v>2</v>
       </c>
     </row>
@@ -2002,7 +2039,7 @@
       <c r="K15" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="19">
         <v>2</v>
       </c>
     </row>
@@ -2034,7 +2071,7 @@
       <c r="K16" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="L16" s="33">
+      <c r="L16" s="19">
         <v>2</v>
       </c>
     </row>
@@ -2066,7 +2103,7 @@
       <c r="K17" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="L17" s="33">
+      <c r="L17" s="19">
         <v>2</v>
       </c>
     </row>
@@ -2098,7 +2135,7 @@
       <c r="K18" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="19">
         <v>2</v>
       </c>
     </row>
@@ -2130,7 +2167,7 @@
       <c r="K19" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="19">
         <v>2</v>
       </c>
     </row>
@@ -2162,27 +2199,27 @@
       <c r="K20" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="L20" s="33">
+      <c r="L20" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:25" s="32" customFormat="1">
+    <row r="21" spans="1:25">
       <c r="A21" s="12" t="s">
         <v>157</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="48"/>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="14" t="s">
@@ -2210,7 +2247,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
-      <c r="L22" s="33">
+      <c r="L22" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2240,7 +2277,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
-      <c r="L23" s="33">
+      <c r="L23" s="19">
         <v>3</v>
       </c>
       <c r="X23" t="s">
@@ -2276,7 +2313,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
       <c r="K24" s="14"/>
-      <c r="L24" s="33">
+      <c r="L24" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2306,7 +2343,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
-      <c r="L25" s="33">
+      <c r="L25" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2336,7 +2373,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
-      <c r="L26" s="33">
+      <c r="L26" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2366,7 +2403,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
-      <c r="L27" s="33">
+      <c r="L27" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2396,7 +2433,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
-      <c r="L28" s="33">
+      <c r="L28" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2426,7 +2463,7 @@
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
-      <c r="L29" s="33">
+      <c r="L29" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2456,7 +2493,7 @@
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
-      <c r="L30" s="33">
+      <c r="L30" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2486,7 +2523,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="33">
+      <c r="L31" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2508,7 +2545,7 @@
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H32" s="14">
         <v>3</v>
@@ -2516,7 +2553,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
-      <c r="L32" s="33">
+      <c r="L32" s="19">
         <v>3</v>
       </c>
       <c r="X32" t="s">
@@ -2539,10 +2576,12 @@
       <c r="D33" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E33" s="14"/>
+      <c r="E33" s="14" t="s">
+        <v>243</v>
+      </c>
       <c r="F33" s="14"/>
       <c r="G33" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H33" s="14">
         <v>3</v>
@@ -2550,7 +2589,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
       <c r="K33" s="14"/>
-      <c r="L33" s="33">
+      <c r="L33" s="19">
         <v>3</v>
       </c>
       <c r="X33" t="s">
@@ -2573,10 +2612,12 @@
       <c r="D34" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E34" s="14"/>
+      <c r="E34" s="14" t="s">
+        <v>243</v>
+      </c>
       <c r="F34" s="14"/>
       <c r="G34" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H34" s="14">
         <v>3</v>
@@ -2584,7 +2625,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
-      <c r="L34" s="33">
+      <c r="L34" s="19">
         <v>3</v>
       </c>
       <c r="X34" t="s">
@@ -2604,10 +2645,12 @@
       <c r="D35" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="14"/>
+      <c r="E35" s="30" t="s">
+        <v>244</v>
+      </c>
       <c r="F35" s="14"/>
       <c r="G35" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H35" s="14">
         <v>3</v>
@@ -2615,7 +2658,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
-      <c r="L35" s="33">
+      <c r="L35" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2633,11 +2676,11 @@
         <v>148</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>168</v>
+        <v>244</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H36" s="14">
         <v>3</v>
@@ -2645,7 +2688,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
-      <c r="L36" s="33">
+      <c r="L36" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2667,7 +2710,7 @@
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H37" s="14">
         <v>3</v>
@@ -2675,7 +2718,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
-      <c r="L37" s="33">
+      <c r="L37" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2697,7 +2740,7 @@
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H38" s="14">
         <v>3</v>
@@ -2705,7 +2748,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
-      <c r="L38" s="33">
+      <c r="L38" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2727,7 +2770,7 @@
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H39" s="14">
         <v>3</v>
@@ -2735,7 +2778,7 @@
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
-      <c r="L39" s="33">
+      <c r="L39" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2752,14 +2795,20 @@
       <c r="D40" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E40" s="14"/>
+      <c r="E40" s="14" t="s">
+        <v>243</v>
+      </c>
       <c r="F40" s="14"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="14"/>
+      <c r="G40" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="H40" s="14">
+        <v>3</v>
+      </c>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
-      <c r="L40" s="33">
+      <c r="L40" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2781,7 +2830,7 @@
       </c>
       <c r="F41" s="14"/>
       <c r="G41" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H41" s="14">
         <v>3</v>
@@ -2789,7 +2838,7 @@
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
-      <c r="L41" s="33">
+      <c r="L41" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2811,7 +2860,7 @@
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H42" s="14">
         <v>3</v>
@@ -2819,7 +2868,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
-      <c r="L42" s="33">
+      <c r="L42" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2841,7 +2890,7 @@
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H43" s="14">
         <v>3</v>
@@ -2849,7 +2898,7 @@
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
-      <c r="L43" s="33">
+      <c r="L43" s="19">
         <v>3</v>
       </c>
     </row>
@@ -2871,7 +2920,7 @@
       </c>
       <c r="F44" s="14"/>
       <c r="G44" s="17" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="H44" s="14">
         <v>3</v>
@@ -2879,7 +2928,7 @@
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
       <c r="K44" s="14"/>
-      <c r="L44" s="33">
+      <c r="L44" s="19">
         <v>3</v>
       </c>
       <c r="X44" t="s">
@@ -2891,16 +2940,16 @@
         <v>173</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="48"/>
     </row>
     <row r="46" spans="1:25">
       <c r="A46" s="14" t="s">
@@ -2926,7 +2975,7 @@
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
       <c r="K46" s="14"/>
-      <c r="L46" s="33">
+      <c r="L46" s="19">
         <v>4</v>
       </c>
     </row>
@@ -2942,7 +2991,7 @@
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
       <c r="K47" s="14"/>
-      <c r="L47" s="33">
+      <c r="L47" s="19">
         <v>4</v>
       </c>
     </row>
@@ -2951,16 +3000,16 @@
         <v>233</v>
       </c>
       <c r="B48" s="13"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="45"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="48"/>
       <c r="X48" s="5" t="s">
         <v>13</v>
       </c>
@@ -2989,7 +3038,7 @@
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
-      <c r="L49" s="33">
+      <c r="L49" s="19">
         <v>3</v>
       </c>
       <c r="X49" t="s">
@@ -3020,7 +3069,7 @@
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
-      <c r="L50" s="33">
+      <c r="L50" s="19">
         <v>3</v>
       </c>
       <c r="X50" t="s">
@@ -3028,92 +3077,54 @@
       </c>
     </row>
     <row r="51" spans="1:24">
-      <c r="A51" s="34"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
+      <c r="A51" s="20"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
       <c r="X51" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
-      <c r="A52" s="34"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
-      <c r="X52" t="s">
+    <row r="52" spans="1:24" s="5" customFormat="1">
+      <c r="A52" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="X52" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:24">
-      <c r="A53" s="34"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35" t="s">
+      <c r="A53" s="20"/>
+      <c r="C53" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="37"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
       <c r="X53" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:24">
-      <c r="A54" s="34"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="35" t="s">
+      <c r="A54" s="20"/>
+      <c r="C54" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="37"/>
-      <c r="L54" s="37"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
       <c r="X54" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:24">
-      <c r="A55" s="34"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35" t="s">
+      <c r="A55" s="20"/>
+      <c r="C55" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="37"/>
-      <c r="L55" s="37"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
       <c r="R55" t="s">
         <v>66</v>
       </c>
@@ -3128,20 +3139,12 @@
       </c>
     </row>
     <row r="56" spans="1:24">
-      <c r="A56" s="34"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35" t="s">
+      <c r="A56" s="20"/>
+      <c r="C56" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="37"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
       <c r="R56" t="s">
         <v>68</v>
       </c>
@@ -3156,18 +3159,9 @@
       </c>
     </row>
     <row r="57" spans="1:24">
-      <c r="A57" s="34"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="36"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="37"/>
+      <c r="A57" s="20"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
       <c r="R57" t="s">
         <v>70</v>
       </c>
@@ -3179,20 +3173,12 @@
       </c>
     </row>
     <row r="58" spans="1:24">
-      <c r="A58" s="34"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35" t="s">
+      <c r="A58" s="20"/>
+      <c r="C58" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="36"/>
-      <c r="K58" s="37"/>
-      <c r="L58" s="37"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
       <c r="R58" t="s">
         <v>60</v>
       </c>
@@ -3211,20 +3197,12 @@
       </c>
     </row>
     <row r="59" spans="1:24">
-      <c r="A59" s="34"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35" t="s">
+      <c r="A59" s="20"/>
+      <c r="C59" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
-      <c r="K59" s="37"/>
-      <c r="L59" s="42"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="26"/>
       <c r="R59" t="s">
         <v>59</v>
       </c>
@@ -3243,20 +3221,12 @@
       </c>
     </row>
     <row r="60" spans="1:24">
-      <c r="A60" s="34"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="35" t="s">
+      <c r="A60" s="20"/>
+      <c r="C60" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="36"/>
-      <c r="J60" s="36"/>
-      <c r="K60" s="37"/>
-      <c r="L60" s="37"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
       <c r="R60" t="s">
         <v>61</v>
       </c>
@@ -3271,18 +3241,9 @@
       </c>
     </row>
     <row r="61" spans="1:24">
-      <c r="A61" s="34"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="36"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="37"/>
+      <c r="A61" s="20"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
       <c r="R61" t="s">
         <v>63</v>
       </c>
@@ -3301,20 +3262,12 @@
       </c>
     </row>
     <row r="62" spans="1:24">
-      <c r="A62" s="34"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35" t="s">
+      <c r="A62" s="20"/>
+      <c r="C62" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="36"/>
-      <c r="J62" s="36"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="37"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
       <c r="R62" t="s">
         <v>64</v>
       </c>
@@ -3333,20 +3286,12 @@
       </c>
     </row>
     <row r="63" spans="1:24">
-      <c r="A63" s="34"/>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35" t="s">
+      <c r="A63" s="20"/>
+      <c r="C63" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="36"/>
-      <c r="J63" s="36"/>
-      <c r="K63" s="37"/>
-      <c r="L63" s="37"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
       <c r="R63" t="s">
         <v>65</v>
       </c>
@@ -3365,20 +3310,12 @@
       </c>
     </row>
     <row r="64" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A64" s="34"/>
-      <c r="B64" s="35"/>
-      <c r="C64" s="35" t="s">
+      <c r="A64" s="20"/>
+      <c r="C64" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="36"/>
-      <c r="K64" s="37"/>
-      <c r="L64" s="37"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
       <c r="R64" s="1" t="s">
         <v>10</v>
       </c>
@@ -3396,37 +3333,20 @@
       </c>
     </row>
     <row r="65" spans="1:24">
-      <c r="A65" s="34"/>
-      <c r="B65" s="35"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="36"/>
-      <c r="I65" s="36"/>
-      <c r="J65" s="36"/>
-      <c r="K65" s="37"/>
-      <c r="L65" s="37"/>
+      <c r="A65" s="20"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
       <c r="X65">
         <v>1.2768999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:24">
-      <c r="A66" s="34"/>
-      <c r="B66" s="35"/>
-      <c r="C66" s="35" t="s">
+      <c r="A66" s="20"/>
+      <c r="C66" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="36"/>
-      <c r="I66" s="36"/>
-      <c r="J66" s="36"/>
-      <c r="K66" s="37"/>
-      <c r="L66" s="37"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
       <c r="R66" t="s">
         <v>42</v>
       </c>
@@ -3439,20 +3359,12 @@
       </c>
     </row>
     <row r="67" spans="1:24">
-      <c r="A67" s="34"/>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35" t="s">
+      <c r="A67" s="20"/>
+      <c r="C67" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="36"/>
-      <c r="J67" s="36"/>
-      <c r="K67" s="37"/>
-      <c r="L67" s="37"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
       <c r="R67" t="s">
         <v>44</v>
       </c>
@@ -3465,20 +3377,12 @@
       </c>
     </row>
     <row r="68" spans="1:24">
-      <c r="A68" s="34"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35" t="s">
+      <c r="A68" s="20"/>
+      <c r="C68" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="36"/>
-      <c r="K68" s="37"/>
-      <c r="L68" s="37"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
       <c r="R68" t="s">
         <v>45</v>
       </c>
@@ -3491,18 +3395,9 @@
       </c>
     </row>
     <row r="69" spans="1:24">
-      <c r="A69" s="34"/>
-      <c r="B69" s="35"/>
-      <c r="C69" s="35"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="36"/>
-      <c r="I69" s="36"/>
-      <c r="J69" s="36"/>
-      <c r="K69" s="37"/>
-      <c r="L69" s="37"/>
+      <c r="A69" s="20"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
       <c r="R69" t="s">
         <v>46</v>
       </c>
@@ -3515,20 +3410,12 @@
       </c>
     </row>
     <row r="70" spans="1:24">
-      <c r="A70" s="34"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36" t="s">
+      <c r="A70" s="20"/>
+      <c r="I70" t="s">
         <v>27</v>
       </c>
-      <c r="J70" s="36"/>
-      <c r="K70" s="37"/>
-      <c r="L70" s="37"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
       <c r="R70" t="s">
         <v>47</v>
       </c>
@@ -3541,20 +3428,12 @@
       </c>
     </row>
     <row r="71" spans="1:24">
-      <c r="A71" s="34"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="35"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="36"/>
-      <c r="I71" s="36" t="s">
+      <c r="A71" s="20"/>
+      <c r="I71" t="s">
         <v>27</v>
       </c>
-      <c r="J71" s="36"/>
-      <c r="K71" s="37"/>
-      <c r="L71" s="37"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="21"/>
       <c r="R71" t="s">
         <v>48</v>
       </c>
@@ -3567,20 +3446,12 @@
       </c>
     </row>
     <row r="72" spans="1:24">
-      <c r="A72" s="34"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="36"/>
-      <c r="I72" s="36" t="s">
+      <c r="A72" s="20"/>
+      <c r="I72" t="s">
         <v>27</v>
       </c>
-      <c r="J72" s="36"/>
-      <c r="K72" s="37"/>
-      <c r="L72" s="37"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="21"/>
       <c r="R72" t="s">
         <v>49</v>
       </c>
@@ -3593,20 +3464,12 @@
       </c>
     </row>
     <row r="73" spans="1:24">
-      <c r="A73" s="34"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="35"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="36" t="s">
+      <c r="A73" s="20"/>
+      <c r="I73" t="s">
         <v>27</v>
       </c>
-      <c r="J73" s="36"/>
-      <c r="K73" s="37"/>
-      <c r="L73" s="37"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
       <c r="R73" t="s">
         <v>50</v>
       </c>
@@ -3619,95 +3482,63 @@
       </c>
     </row>
     <row r="74" spans="1:24">
-      <c r="A74" s="34"/>
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="36"/>
-      <c r="J74" s="36"/>
-      <c r="K74" s="37"/>
-      <c r="L74" s="37"/>
+      <c r="A74" s="20"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
     </row>
     <row r="75" spans="1:24">
-      <c r="A75" s="34"/>
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="36"/>
-      <c r="I75" s="36" t="s">
+      <c r="A75" s="20"/>
+      <c r="I75" t="s">
         <v>28</v>
       </c>
-      <c r="J75" s="36"/>
-      <c r="K75" s="37"/>
-      <c r="L75" s="37"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
     </row>
     <row r="76" spans="1:24">
-      <c r="A76" s="34"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="36"/>
-      <c r="I76" s="36"/>
-      <c r="J76" s="36"/>
-      <c r="K76" s="37"/>
-      <c r="L76" s="37"/>
+      <c r="A76" s="20"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="21"/>
     </row>
     <row r="77" spans="1:24">
-      <c r="A77" s="34"/>
-      <c r="B77" s="35"/>
-      <c r="C77" s="35"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="36"/>
-      <c r="J77" s="36"/>
-      <c r="K77" s="37"/>
-      <c r="L77" s="37"/>
+      <c r="A77" s="20"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="21"/>
     </row>
     <row r="78" spans="1:24">
-      <c r="A78" s="38" t="s">
+      <c r="A78" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
-      <c r="F78" s="40"/>
-      <c r="G78" s="40"/>
-      <c r="H78" s="40"/>
-      <c r="I78" s="40" t="s">
+      <c r="B78" s="23"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="J78" s="40"/>
-      <c r="K78" s="41"/>
-      <c r="L78" s="41"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="25"/>
+      <c r="L78" s="25"/>
+    </row>
+    <row r="79" spans="1:24">
+      <c r="A79" s="32"/>
     </row>
     <row r="82" spans="12:21">
-      <c r="L82" s="29" t="s">
+      <c r="L82" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="M82" s="30"/>
-      <c r="N82" s="31" t="s">
+      <c r="M82" s="44"/>
+      <c r="N82" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="O82" s="31"/>
-      <c r="P82" s="31"/>
-      <c r="Q82" s="31"/>
-      <c r="R82" s="31"/>
-      <c r="S82" s="31"/>
-      <c r="T82" s="31"/>
+      <c r="O82" s="45"/>
+      <c r="P82" s="45"/>
+      <c r="Q82" s="45"/>
+      <c r="R82" s="45"/>
+      <c r="S82" s="45"/>
+      <c r="T82" s="45"/>
     </row>
     <row r="83" spans="12:21">
       <c r="L83" s="10" t="s">
@@ -4310,10 +4141,10 @@
       <c r="O102" s="8">
         <v>355.6</v>
       </c>
-      <c r="P102" s="19"/>
-      <c r="Q102" s="20"/>
-      <c r="R102" s="20"/>
-      <c r="S102" s="21"/>
+      <c r="P102" s="34"/>
+      <c r="Q102" s="35"/>
+      <c r="R102" s="35"/>
+      <c r="S102" s="36"/>
       <c r="T102" s="7" t="s">
         <v>174</v>
       </c>
@@ -4331,10 +4162,10 @@
       <c r="O103" s="8">
         <v>406.4</v>
       </c>
-      <c r="P103" s="22"/>
-      <c r="Q103" s="23"/>
-      <c r="R103" s="23"/>
-      <c r="S103" s="24"/>
+      <c r="P103" s="37"/>
+      <c r="Q103" s="38"/>
+      <c r="R103" s="38"/>
+      <c r="S103" s="39"/>
       <c r="T103" s="7" t="s">
         <v>174</v>
       </c>
@@ -4352,10 +4183,10 @@
       <c r="O104" s="8">
         <v>457.2</v>
       </c>
-      <c r="P104" s="22"/>
-      <c r="Q104" s="23"/>
-      <c r="R104" s="23"/>
-      <c r="S104" s="24"/>
+      <c r="P104" s="37"/>
+      <c r="Q104" s="38"/>
+      <c r="R104" s="38"/>
+      <c r="S104" s="39"/>
       <c r="T104" s="7" t="s">
         <v>174</v>
       </c>
@@ -4373,10 +4204,10 @@
       <c r="O105" s="8">
         <v>508</v>
       </c>
-      <c r="P105" s="22"/>
-      <c r="Q105" s="23"/>
-      <c r="R105" s="23"/>
-      <c r="S105" s="24"/>
+      <c r="P105" s="37"/>
+      <c r="Q105" s="38"/>
+      <c r="R105" s="38"/>
+      <c r="S105" s="39"/>
       <c r="T105" s="7" t="s">
         <v>174</v>
       </c>
@@ -4394,10 +4225,10 @@
       <c r="O106" s="8">
         <v>609.6</v>
       </c>
-      <c r="P106" s="25"/>
-      <c r="Q106" s="26"/>
-      <c r="R106" s="26"/>
-      <c r="S106" s="27"/>
+      <c r="P106" s="40"/>
+      <c r="Q106" s="41"/>
+      <c r="R106" s="41"/>
+      <c r="S106" s="42"/>
       <c r="T106" s="7" t="s">
         <v>174</v>
       </c>
@@ -4564,8 +4395,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="P102:S106"/>
-    <mergeCell ref="A1:G1"/>
     <mergeCell ref="L82:M82"/>
     <mergeCell ref="N82:T82"/>
     <mergeCell ref="C3:L3"/>

</xml_diff>

<commit_message>
Medir peças multicorpos e inserir em propCutList
</commit_message>
<xml_diff>
--- a/BdaC_ProAtiv.xlsx
+++ b/BdaC_ProAtiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Projetos4\Desktop\ALESSANDRO\MACRO\Criando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119B0CC4-F498-43C5-8176-0E221D9F7434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EA72E8-DD7C-4BD1-8985-E0BF8320959B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26175" yWindow="1500" windowWidth="17100" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -976,7 +976,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="44"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1229,7 +1229,6 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1279,6 +1278,7 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1580,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1608,20 +1608,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
@@ -1674,16 +1674,16 @@
       <c r="B3" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="48"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="14" t="s">
@@ -1968,19 +1968,19 @@
       <c r="B13" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="48"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="47"/>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="48" t="s">
         <v>131</v>
       </c>
       <c r="B14" s="15" t="s">
@@ -2210,16 +2210,16 @@
       <c r="B21" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C21" s="46"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="48"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="47"/>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="14" t="s">
@@ -2940,16 +2940,16 @@
         <v>173</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="48"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="47"/>
     </row>
     <row r="46" spans="1:25">
       <c r="A46" s="14" t="s">
@@ -3000,16 +3000,16 @@
         <v>233</v>
       </c>
       <c r="B48" s="13"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="48"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="47"/>
       <c r="X48" s="5" t="s">
         <v>13</v>
       </c>
@@ -3523,22 +3523,22 @@
       <c r="L78" s="25"/>
     </row>
     <row r="79" spans="1:24">
-      <c r="A79" s="32"/>
+      <c r="A79" s="31"/>
     </row>
     <row r="82" spans="12:21">
-      <c r="L82" s="43" t="s">
+      <c r="L82" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="M82" s="44"/>
-      <c r="N82" s="45" t="s">
+      <c r="M82" s="43"/>
+      <c r="N82" s="44" t="s">
         <v>177</v>
       </c>
-      <c r="O82" s="45"/>
-      <c r="P82" s="45"/>
-      <c r="Q82" s="45"/>
-      <c r="R82" s="45"/>
-      <c r="S82" s="45"/>
-      <c r="T82" s="45"/>
+      <c r="O82" s="44"/>
+      <c r="P82" s="44"/>
+      <c r="Q82" s="44"/>
+      <c r="R82" s="44"/>
+      <c r="S82" s="44"/>
+      <c r="T82" s="44"/>
     </row>
     <row r="83" spans="12:21">
       <c r="L83" s="10" t="s">
@@ -4141,10 +4141,10 @@
       <c r="O102" s="8">
         <v>355.6</v>
       </c>
-      <c r="P102" s="34"/>
-      <c r="Q102" s="35"/>
-      <c r="R102" s="35"/>
-      <c r="S102" s="36"/>
+      <c r="P102" s="33"/>
+      <c r="Q102" s="34"/>
+      <c r="R102" s="34"/>
+      <c r="S102" s="35"/>
       <c r="T102" s="7" t="s">
         <v>174</v>
       </c>
@@ -4162,10 +4162,10 @@
       <c r="O103" s="8">
         <v>406.4</v>
       </c>
-      <c r="P103" s="37"/>
-      <c r="Q103" s="38"/>
-      <c r="R103" s="38"/>
-      <c r="S103" s="39"/>
+      <c r="P103" s="36"/>
+      <c r="Q103" s="37"/>
+      <c r="R103" s="37"/>
+      <c r="S103" s="38"/>
       <c r="T103" s="7" t="s">
         <v>174</v>
       </c>
@@ -4183,10 +4183,10 @@
       <c r="O104" s="8">
         <v>457.2</v>
       </c>
-      <c r="P104" s="37"/>
-      <c r="Q104" s="38"/>
-      <c r="R104" s="38"/>
-      <c r="S104" s="39"/>
+      <c r="P104" s="36"/>
+      <c r="Q104" s="37"/>
+      <c r="R104" s="37"/>
+      <c r="S104" s="38"/>
       <c r="T104" s="7" t="s">
         <v>174</v>
       </c>
@@ -4204,10 +4204,10 @@
       <c r="O105" s="8">
         <v>508</v>
       </c>
-      <c r="P105" s="37"/>
-      <c r="Q105" s="38"/>
-      <c r="R105" s="38"/>
-      <c r="S105" s="39"/>
+      <c r="P105" s="36"/>
+      <c r="Q105" s="37"/>
+      <c r="R105" s="37"/>
+      <c r="S105" s="38"/>
       <c r="T105" s="7" t="s">
         <v>174</v>
       </c>
@@ -4225,10 +4225,10 @@
       <c r="O106" s="8">
         <v>609.6</v>
       </c>
-      <c r="P106" s="40"/>
-      <c r="Q106" s="41"/>
-      <c r="R106" s="41"/>
-      <c r="S106" s="42"/>
+      <c r="P106" s="39"/>
+      <c r="Q106" s="40"/>
+      <c r="R106" s="40"/>
+      <c r="S106" s="41"/>
       <c r="T106" s="7" t="s">
         <v>174</v>
       </c>

</xml_diff>